<commit_message>
adding apb sub sytem.
</commit_message>
<xml_diff>
--- a/my1stProject/apb_subsystem/apb_subsustem_design_arch.xlsx
+++ b/my1stProject/apb_subsystem/apb_subsustem_design_arch.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SoC\demo\apb_subsystem\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="3" r:id="rId1"/>
@@ -26,8 +21,8 @@
     <definedName name="vsupply">#REF!</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -40,7 +35,7 @@
     <author>shashank</author>
   </authors>
   <commentList>
-    <comment ref="D27" authorId="0" shapeId="0">
+    <comment ref="D27" authorId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D41" authorId="0" shapeId="0">
+    <comment ref="D41" authorId="0">
       <text>
         <r>
           <rPr>
@@ -68,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D163" authorId="0" shapeId="0">
+    <comment ref="D163" authorId="0">
       <text>
         <r>
           <rPr>
@@ -92,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D164" authorId="0" shapeId="0">
+    <comment ref="D164" authorId="0">
       <text>
         <r>
           <rPr>
@@ -116,7 +111,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D165" authorId="0" shapeId="0">
+    <comment ref="D165" authorId="0">
       <text>
         <r>
           <rPr>
@@ -140,7 +135,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D166" authorId="0" shapeId="0">
+    <comment ref="D166" authorId="0">
       <text>
         <r>
           <rPr>
@@ -169,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="400">
   <si>
     <t>Target</t>
   </si>
@@ -1382,9 +1377,15 @@
     <t>uart</t>
   </si>
   <si>
+    <t>i_uarts</t>
+  </si>
+  <si>
     <t>i_uart_1</t>
   </si>
   <si>
+    <t>uart_1</t>
+  </si>
+  <si>
     <t>i_uartcrosser</t>
   </si>
   <si>
@@ -1473,19 +1474,13 @@
   </si>
   <si>
     <t>irq[14:4]</t>
-  </si>
-  <si>
-    <t>apbbus8</t>
-  </si>
-  <si>
-    <t>../apbmst/apbmst.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2563,27 +2558,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="53.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15" customHeight="1">
       <c r="A1" s="96" t="s">
         <v>3</v>
       </c>
@@ -2600,63 +2595,63 @@
       <c r="J1" s="101"/>
       <c r="K1" s="101"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A2" s="98"/>
       <c r="B2" s="99"/>
     </row>
-    <row r="6" spans="1:11" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:11" ht="29.25" thickBot="1">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="5"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="B7" s="7" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:11" ht="29.25" thickBot="1">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="B9" s="8" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:11" ht="29.25" thickBot="1">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="B11" s="8" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:11" ht="29.25" thickBot="1">
       <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="B13" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:11" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:11" ht="29.25" thickBot="1">
       <c r="A15" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="B16" s="9"/>
       <c r="D16" s="2"/>
     </row>
@@ -2671,14 +2666,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" style="10" bestFit="1" customWidth="1"/>
@@ -2693,7 +2688,7 @@
     <col min="11" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75">
       <c r="A1" s="96" t="s">
         <v>272</v>
       </c>
@@ -2705,12 +2700,12 @@
       <c r="E1" s="101"/>
       <c r="F1" s="101"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1">
       <c r="A2" s="98"/>
       <c r="B2" s="99"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1"/>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1">
       <c r="A4" s="26" t="s">
         <v>10</v>
       </c>
@@ -2742,7 +2737,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1">
       <c r="A5" s="21" t="s">
         <v>360</v>
       </c>
@@ -2762,11 +2757,9 @@
       <c r="G5" s="24"/>
       <c r="H5" s="25"/>
       <c r="I5" s="17"/>
-      <c r="J5" s="15" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J5" s="15"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1">
       <c r="A6" s="12" t="s">
         <v>362</v>
       </c>
@@ -2788,7 +2781,7 @@
       <c r="I6" s="17"/>
       <c r="J6" s="15"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>364</v>
       </c>
@@ -2810,9 +2803,9 @@
       <c r="I7" s="17"/>
       <c r="J7" s="15"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1">
       <c r="A8" s="12" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="B8" s="22" t="s">
         <v>358</v>
@@ -2832,9 +2825,9 @@
       <c r="I8" s="17"/>
       <c r="J8" s="15"/>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15.75" thickBot="1">
       <c r="A9" s="12" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B9" s="22" t="s">
         <v>358</v>
@@ -2843,7 +2836,7 @@
         <v>359</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="E9" s="23">
         <v>1.2</v>
@@ -2854,9 +2847,9 @@
       <c r="I9" s="17"/>
       <c r="J9" s="15"/>
     </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10">
       <c r="A10" s="18" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B10" s="22" t="s">
         <v>358</v>
@@ -2865,7 +2858,7 @@
         <v>359</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="E10" s="23">
         <v>1.2</v>
@@ -2875,28 +2868,18 @@
       <c r="H10" s="20"/>
       <c r="I10" s="18"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>371</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>358</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>359</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>398</v>
-      </c>
-      <c r="E11" s="23">
-        <v>1.2</v>
-      </c>
+    <row r="11" spans="1:10">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="19"/>
       <c r="F11" s="19"/>
       <c r="G11" s="20"/>
       <c r="H11" s="20"/>
       <c r="I11" s="18"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="18"/>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
@@ -2907,7 +2890,7 @@
       <c r="H12" s="20"/>
       <c r="I12" s="18"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
@@ -2918,7 +2901,7 @@
       <c r="H13" s="20"/>
       <c r="I13" s="18"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
@@ -2940,14 +2923,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
@@ -2961,7 +2944,7 @@
     <col min="11" max="11" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75">
       <c r="A1" s="96" t="s">
         <v>274</v>
       </c>
@@ -2973,12 +2956,12 @@
       <c r="E1" s="101"/>
       <c r="F1" s="101"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1">
       <c r="A2" s="98"/>
       <c r="B2" s="99"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1">
       <c r="A5" s="30" t="s">
         <v>1</v>
       </c>
@@ -2998,163 +2981,163 @@
         <v>295</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
         <v>360</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>362</v>
       </c>
       <c r="B7" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C7" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="D7" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>364</v>
       </c>
       <c r="B8" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C8" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="D8" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B9" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C9" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="D9" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B10" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C10" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="D10" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>362</v>
       </c>
       <c r="B11" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C11" t="s">
         <v>364</v>
       </c>
       <c r="D11" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>362</v>
       </c>
       <c r="B12" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="C12" t="s">
         <v>364</v>
       </c>
       <c r="D12" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>362</v>
       </c>
       <c r="B13" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="C13" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="D13" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>362</v>
       </c>
       <c r="B14" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="C14" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D14" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B15" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="C15" t="s">
+        <v>370</v>
+      </c>
+      <c r="D15" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
         <v>368</v>
       </c>
-      <c r="D15" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>367</v>
-      </c>
       <c r="B16" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="C16" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="D16" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -3162,7 +3145,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -3181,14 +3164,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.140625" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
@@ -3198,7 +3181,7 @@
     <col min="6" max="6" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75">
       <c r="A1" s="96" t="s">
         <v>276</v>
       </c>
@@ -3212,11 +3195,11 @@
       <c r="G1" s="91"/>
       <c r="H1" s="91"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1">
       <c r="A2" s="98"/>
       <c r="B2" s="99"/>
     </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="15.75" thickBot="1">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -3224,7 +3207,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="15.75" thickBot="1">
       <c r="A5" s="30" t="s">
         <v>299</v>
       </c>
@@ -3244,121 +3227,121 @@
         <v>309</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B6" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="C6" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="D6" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B7" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="C7" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="D7" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>364</v>
       </c>
       <c r="B8" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="E8" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>362</v>
       </c>
       <c r="B9" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="E9" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>364</v>
       </c>
       <c r="B10" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="E10" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>364</v>
       </c>
       <c r="B11" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="E11" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>364</v>
       </c>
       <c r="B12" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="E12" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>364</v>
       </c>
       <c r="B13" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="E13" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>364</v>
       </c>
       <c r="B14" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="E14" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>364</v>
       </c>
       <c r="B15" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="E15" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -3370,14 +3353,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:F179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F154" sqref="F154"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="26.28515625" customWidth="1" collapsed="1"/>
@@ -3387,7 +3370,7 @@
     <col min="6" max="6" width="93.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="B2" s="34" t="s">
         <v>13</v>
       </c>
@@ -3404,21 +3387,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="B3" s="38"/>
       <c r="C3" s="39"/>
       <c r="D3" s="39"/>
       <c r="E3" s="39"/>
       <c r="F3" s="40"/>
     </row>
-    <row r="4" spans="1:6" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="41" customFormat="1">
       <c r="B4" s="42"/>
       <c r="C4" s="43"/>
       <c r="D4" s="43"/>
       <c r="E4" s="43"/>
       <c r="F4" s="44"/>
     </row>
-    <row r="5" spans="1:6" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="41" customFormat="1">
       <c r="B5" s="45" t="s">
         <v>18</v>
       </c>
@@ -3431,7 +3414,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="41" customFormat="1">
       <c r="B6" s="45" t="s">
         <v>21</v>
       </c>
@@ -3444,7 +3427,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="41" customFormat="1">
       <c r="B7" s="45" t="s">
         <v>24</v>
       </c>
@@ -3457,7 +3440,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="51" customFormat="1">
       <c r="A8" s="48"/>
       <c r="B8" s="49" t="s">
         <v>27</v>
@@ -3471,7 +3454,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="51" customFormat="1">
       <c r="A9" s="48"/>
       <c r="B9" s="49" t="s">
         <v>313</v>
@@ -3485,7 +3468,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="51" customFormat="1">
       <c r="A10" s="48"/>
       <c r="B10" s="49" t="s">
         <v>32</v>
@@ -3499,7 +3482,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="51" customFormat="1">
       <c r="A11" s="48"/>
       <c r="B11" s="49" t="s">
         <v>35</v>
@@ -3513,7 +3496,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="53"/>
       <c r="B12" s="45" t="s">
         <v>38</v>
@@ -3527,7 +3510,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15" customHeight="1">
       <c r="B13" s="54" t="s">
         <v>314</v>
       </c>
@@ -3540,7 +3523,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="B14" s="45" t="s">
         <v>43</v>
       </c>
@@ -3553,7 +3536,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="B15" s="56" t="s">
         <v>46</v>
       </c>
@@ -3566,7 +3549,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="B16" s="56" t="s">
         <v>49</v>
       </c>
@@ -3579,7 +3562,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="58"/>
       <c r="B17" s="45" t="s">
         <v>52</v>
@@ -3593,7 +3576,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="59"/>
       <c r="B18" s="45" t="s">
         <v>55</v>
@@ -3607,7 +3590,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="59"/>
       <c r="B19" s="45" t="s">
         <v>58</v>
@@ -3619,7 +3602,7 @@
       <c r="E19" s="104"/>
       <c r="F19" s="57"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="59"/>
       <c r="B20" s="45" t="s">
         <v>60</v>
@@ -3631,7 +3614,7 @@
       <c r="E20" s="104"/>
       <c r="F20" s="57"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="B21" s="45" t="s">
         <v>62</v>
       </c>
@@ -3641,13 +3624,13 @@
       <c r="D21" s="102"/>
       <c r="E21" s="104"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="B22" s="60"/>
       <c r="C22" s="55"/>
       <c r="D22" s="102"/>
       <c r="E22" s="104"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="B23" s="54" t="s">
         <v>315</v>
       </c>
@@ -3660,7 +3643,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="53"/>
       <c r="B24" s="61" t="s">
         <v>66</v>
@@ -3674,7 +3657,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="B25" s="54" t="s">
         <v>69</v>
       </c>
@@ -3687,7 +3670,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="53"/>
       <c r="B26" s="62" t="s">
         <v>72</v>
@@ -3701,7 +3684,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="B27" s="62" t="s">
         <v>75</v>
       </c>
@@ -3716,7 +3699,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="53"/>
       <c r="B28" s="62" t="s">
         <v>78</v>
@@ -3728,7 +3711,7 @@
       <c r="E28" s="104"/>
       <c r="F28" s="57"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="59"/>
       <c r="B29" s="54" t="s">
         <v>80</v>
@@ -3742,7 +3725,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="59"/>
       <c r="B30" s="54" t="s">
         <v>316</v>
@@ -3754,7 +3737,7 @@
       <c r="E30" s="104"/>
       <c r="F30" s="57"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="59"/>
       <c r="B31" s="45" t="s">
         <v>84</v>
@@ -3768,7 +3751,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="59"/>
       <c r="B32" s="45" t="s">
         <v>87</v>
@@ -3780,7 +3763,7 @@
       <c r="E32" s="104"/>
       <c r="F32" s="57"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="59"/>
       <c r="B33" s="45" t="s">
         <v>89</v>
@@ -3792,7 +3775,7 @@
       <c r="E33" s="104"/>
       <c r="F33" s="57"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="59"/>
       <c r="B34" s="45" t="s">
         <v>91</v>
@@ -3804,7 +3787,7 @@
       <c r="E34" s="104"/>
       <c r="F34" s="57"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="59"/>
       <c r="B35" s="62" t="s">
         <v>93</v>
@@ -3816,7 +3799,7 @@
       <c r="E35" s="104"/>
       <c r="F35" s="57"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="B36" s="62" t="s">
         <v>95</v>
       </c>
@@ -3827,14 +3810,14 @@
       <c r="E36" s="104"/>
       <c r="F36" s="57"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="B37" s="62"/>
       <c r="C37" s="55"/>
       <c r="D37" s="106"/>
       <c r="E37" s="104"/>
       <c r="F37" s="57"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="B38" s="54" t="s">
         <v>317</v>
       </c>
@@ -3847,7 +3830,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="B39" s="54" t="s">
         <v>318</v>
       </c>
@@ -3860,7 +3843,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40" s="59"/>
       <c r="B40" s="54" t="s">
         <v>319</v>
@@ -3876,7 +3859,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="B41" s="65" t="s">
         <v>320</v>
       </c>
@@ -3891,7 +3874,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42" s="59"/>
       <c r="B42" s="54" t="s">
         <v>321</v>
@@ -3907,7 +3890,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="B43" s="54" t="s">
         <v>322</v>
       </c>
@@ -3920,7 +3903,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="B44" s="54" t="s">
         <v>111</v>
       </c>
@@ -3933,7 +3916,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="B45" s="54" t="s">
         <v>114</v>
       </c>
@@ -3944,14 +3927,14 @@
       <c r="E45" s="104"/>
       <c r="F45" s="57"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="B46" s="54"/>
       <c r="C46" s="66"/>
       <c r="D46" s="109"/>
       <c r="E46" s="104"/>
       <c r="F46" s="57"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="B47" s="45" t="s">
         <v>116</v>
       </c>
@@ -3964,7 +3947,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6">
       <c r="B48" s="45" t="s">
         <v>119</v>
       </c>
@@ -3974,13 +3957,13 @@
       <c r="D48" s="109"/>
       <c r="E48" s="104"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="B49" s="67"/>
       <c r="C49" s="66"/>
       <c r="D49" s="109"/>
       <c r="E49" s="104"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="B50" s="54" t="s">
         <v>121</v>
       </c>
@@ -3993,7 +3976,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6">
       <c r="B51" s="54" t="s">
         <v>124</v>
       </c>
@@ -4006,7 +3989,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="B52" s="54" t="s">
         <v>127</v>
       </c>
@@ -4019,7 +4002,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="B53" s="54" t="s">
         <v>130</v>
       </c>
@@ -4032,7 +4015,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6">
       <c r="B54" s="54" t="s">
         <v>133</v>
       </c>
@@ -4045,7 +4028,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="B55" s="54" t="s">
         <v>136</v>
       </c>
@@ -4058,7 +4041,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6">
       <c r="B56" s="54" t="s">
         <v>139</v>
       </c>
@@ -4071,14 +4054,14 @@
         <v>141</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="B57" s="54"/>
       <c r="C57" s="66"/>
       <c r="D57" s="109"/>
       <c r="E57" s="104"/>
       <c r="F57" s="57"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="A58" s="68"/>
       <c r="B58" s="54" t="s">
         <v>323</v>
@@ -4092,7 +4075,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="A59" s="69"/>
       <c r="B59" s="54" t="s">
         <v>144</v>
@@ -4106,7 +4089,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="A60" s="69"/>
       <c r="B60" s="54" t="s">
         <v>147</v>
@@ -4120,7 +4103,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="A61" s="69"/>
       <c r="B61" s="54" t="s">
         <v>150</v>
@@ -4134,7 +4117,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6">
       <c r="A62" s="69"/>
       <c r="B62" s="54" t="s">
         <v>153</v>
@@ -4148,7 +4131,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="15" customHeight="1">
       <c r="A63" s="70"/>
       <c r="B63" s="54" t="s">
         <v>155</v>
@@ -4162,7 +4145,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6">
       <c r="A64" s="70"/>
       <c r="B64" s="54" t="s">
         <v>324</v>
@@ -4176,7 +4159,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6">
       <c r="A65" s="70"/>
       <c r="B65" s="54" t="s">
         <v>160</v>
@@ -4190,7 +4173,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6">
       <c r="A66" s="70"/>
       <c r="B66" s="54" t="s">
         <v>163</v>
@@ -4204,7 +4187,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6">
       <c r="A67" s="70"/>
       <c r="B67" s="54" t="s">
         <v>166</v>
@@ -4218,7 +4201,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6">
       <c r="B68" s="54" t="s">
         <v>169</v>
       </c>
@@ -4231,7 +4214,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6">
       <c r="B69" s="54" t="s">
         <v>172</v>
       </c>
@@ -4244,7 +4227,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6">
       <c r="B70" s="54" t="s">
         <v>175</v>
       </c>
@@ -4255,7 +4238,7 @@
       <c r="E70" s="71"/>
       <c r="F70" s="57"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6">
       <c r="B71" s="54" t="s">
         <v>177</v>
       </c>
@@ -4268,28 +4251,28 @@
         <v>179</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6">
       <c r="B72" s="74"/>
       <c r="C72" s="75"/>
       <c r="D72" s="76"/>
       <c r="E72" s="77"/>
       <c r="F72" s="57"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6">
       <c r="B73" s="74"/>
       <c r="C73" s="75"/>
       <c r="D73" s="76"/>
       <c r="E73" s="77"/>
       <c r="F73" s="57"/>
     </row>
-    <row r="74" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" ht="15.75" thickBot="1">
       <c r="B74" s="74"/>
       <c r="C74" s="75"/>
       <c r="D74" s="76"/>
       <c r="E74" s="77"/>
       <c r="F74" s="57"/>
     </row>
-    <row r="75" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" ht="15.75" thickBot="1">
       <c r="A75" s="53" t="s">
         <v>180</v>
       </c>
@@ -4303,7 +4286,7 @@
       <c r="E75" s="77"/>
       <c r="F75" s="57"/>
     </row>
-    <row r="76" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" ht="15.75" thickBot="1">
       <c r="B76" s="80" t="s">
         <v>325</v>
       </c>
@@ -4314,7 +4297,7 @@
       <c r="E76" s="77"/>
       <c r="F76" s="57"/>
     </row>
-    <row r="77" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" ht="15.75" thickBot="1">
       <c r="B77" s="82" t="s">
         <v>326</v>
       </c>
@@ -4325,7 +4308,7 @@
       <c r="E77" s="77"/>
       <c r="F77" s="57"/>
     </row>
-    <row r="78" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" ht="15.75" thickBot="1">
       <c r="B78" s="82" t="s">
         <v>327</v>
       </c>
@@ -4336,14 +4319,14 @@
       <c r="E78" s="77"/>
       <c r="F78" s="57"/>
     </row>
-    <row r="79" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" ht="15.75" thickBot="1">
       <c r="B79" s="82"/>
       <c r="C79" s="81"/>
       <c r="D79" s="76"/>
       <c r="E79" s="77"/>
       <c r="F79" s="57"/>
     </row>
-    <row r="80" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" ht="15.75" thickBot="1">
       <c r="A80" s="53" t="s">
         <v>185</v>
       </c>
@@ -4357,7 +4340,7 @@
       <c r="E80" s="77"/>
       <c r="F80" s="57"/>
     </row>
-    <row r="81" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" ht="15.75" thickBot="1">
       <c r="B81" s="80" t="s">
         <v>329</v>
       </c>
@@ -4368,7 +4351,7 @@
       <c r="E81" s="77"/>
       <c r="F81" s="57"/>
     </row>
-    <row r="82" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" ht="15.75" thickBot="1">
       <c r="B82" s="82" t="s">
         <v>330</v>
       </c>
@@ -4379,7 +4362,7 @@
       <c r="E82" s="77"/>
       <c r="F82" s="57"/>
     </row>
-    <row r="83" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" ht="15.75" thickBot="1">
       <c r="B83" s="82" t="s">
         <v>331</v>
       </c>
@@ -4390,14 +4373,14 @@
       <c r="E83" s="77"/>
       <c r="F83" s="57"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6">
       <c r="B84" s="74"/>
       <c r="C84" s="75"/>
       <c r="D84" s="76"/>
       <c r="E84" s="77"/>
       <c r="F84" s="57"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6">
       <c r="A85" s="53" t="s">
         <v>190</v>
       </c>
@@ -4407,7 +4390,7 @@
       <c r="E85" s="77"/>
       <c r="F85" s="57"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6">
       <c r="B86" s="74" t="s">
         <v>191</v>
       </c>
@@ -4418,7 +4401,7 @@
       <c r="E86" s="77"/>
       <c r="F86" s="57"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6">
       <c r="B87" s="74" t="s">
         <v>193</v>
       </c>
@@ -4429,7 +4412,7 @@
       <c r="E87" s="77"/>
       <c r="F87" s="57"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6">
       <c r="B88" s="74" t="s">
         <v>332</v>
       </c>
@@ -4440,7 +4423,7 @@
       <c r="E88" s="77"/>
       <c r="F88" s="57"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6">
       <c r="B89" s="74" t="s">
         <v>196</v>
       </c>
@@ -4451,7 +4434,7 @@
       <c r="E89" s="77"/>
       <c r="F89" s="57"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6">
       <c r="B90" s="74" t="s">
         <v>198</v>
       </c>
@@ -4462,7 +4445,7 @@
       <c r="E90" s="77"/>
       <c r="F90" s="57"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6">
       <c r="B91" s="74" t="s">
         <v>269</v>
       </c>
@@ -4473,7 +4456,7 @@
       <c r="E91" s="77"/>
       <c r="F91" s="57"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6">
       <c r="B92" s="74" t="s">
         <v>201</v>
       </c>
@@ -4484,14 +4467,14 @@
       <c r="E92" s="77"/>
       <c r="F92" s="57"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6">
       <c r="B93" s="74"/>
       <c r="C93" s="75"/>
       <c r="D93" s="76"/>
       <c r="E93" s="77"/>
       <c r="F93" s="57"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6">
       <c r="A94" s="53" t="s">
         <v>203</v>
       </c>
@@ -4501,7 +4484,7 @@
       <c r="E94" s="77"/>
       <c r="F94" s="57"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6">
       <c r="B95" s="74" t="s">
         <v>333</v>
       </c>
@@ -4512,7 +4495,7 @@
       <c r="E95" s="77"/>
       <c r="F95" s="57"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6">
       <c r="B96" s="74" t="s">
         <v>205</v>
       </c>
@@ -4523,7 +4506,7 @@
       <c r="E96" s="77"/>
       <c r="F96" s="57"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6">
       <c r="B97" s="74" t="s">
         <v>207</v>
       </c>
@@ -4534,7 +4517,7 @@
       <c r="E97" s="77"/>
       <c r="F97" s="57"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6">
       <c r="B98" s="74" t="s">
         <v>209</v>
       </c>
@@ -4545,7 +4528,7 @@
       <c r="E98" s="77"/>
       <c r="F98" s="57"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6">
       <c r="B99" s="74" t="s">
         <v>211</v>
       </c>
@@ -4556,7 +4539,7 @@
       <c r="E99" s="77"/>
       <c r="F99" s="57"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6">
       <c r="B100" s="74" t="s">
         <v>213</v>
       </c>
@@ -4567,7 +4550,7 @@
       <c r="E100" s="77"/>
       <c r="F100" s="57"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6">
       <c r="B101" s="74" t="s">
         <v>215</v>
       </c>
@@ -4578,7 +4561,7 @@
       <c r="E101" s="77"/>
       <c r="F101" s="57"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6">
       <c r="B102" s="74" t="s">
         <v>217</v>
       </c>
@@ -4589,7 +4572,7 @@
       <c r="E102" s="77"/>
       <c r="F102" s="57"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6">
       <c r="B103" s="74" t="s">
         <v>219</v>
       </c>
@@ -4600,7 +4583,7 @@
       <c r="E103" s="77"/>
       <c r="F103" s="57"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6">
       <c r="B104" s="74" t="s">
         <v>221</v>
       </c>
@@ -4611,7 +4594,7 @@
       <c r="E104" s="77"/>
       <c r="F104" s="57"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6">
       <c r="B105" s="74" t="s">
         <v>223</v>
       </c>
@@ -4622,7 +4605,7 @@
       <c r="E105" s="77"/>
       <c r="F105" s="57"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6">
       <c r="B106" s="74" t="s">
         <v>334</v>
       </c>
@@ -4633,14 +4616,14 @@
       <c r="E106" s="77"/>
       <c r="F106" s="57"/>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6">
       <c r="B107" s="74"/>
       <c r="C107" s="75"/>
       <c r="D107" s="76"/>
       <c r="E107" s="77"/>
       <c r="F107" s="57"/>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6">
       <c r="A108" s="53" t="s">
         <v>226</v>
       </c>
@@ -4654,7 +4637,7 @@
       <c r="E108" s="77"/>
       <c r="F108" s="57"/>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6">
       <c r="B109" s="74" t="s">
         <v>335</v>
       </c>
@@ -4665,14 +4648,14 @@
       <c r="E109" s="77"/>
       <c r="F109" s="57"/>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6">
       <c r="B110" s="74"/>
       <c r="C110" s="75"/>
       <c r="D110" s="76"/>
       <c r="E110" s="77"/>
       <c r="F110" s="57"/>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6">
       <c r="A111" s="53" t="s">
         <v>230</v>
       </c>
@@ -4682,7 +4665,7 @@
       <c r="E111" s="77"/>
       <c r="F111" s="57"/>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6">
       <c r="B112" s="74" t="s">
         <v>336</v>
       </c>
@@ -4693,7 +4676,7 @@
       <c r="E112" s="77"/>
       <c r="F112" s="57"/>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6">
       <c r="B113" s="74" t="s">
         <v>337</v>
       </c>
@@ -4704,7 +4687,7 @@
       <c r="E113" s="77"/>
       <c r="F113" s="57"/>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6">
       <c r="B114" s="74" t="s">
         <v>338</v>
       </c>
@@ -4715,7 +4698,7 @@
       <c r="E114" s="77"/>
       <c r="F114" s="57"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6">
       <c r="B115" s="74" t="s">
         <v>339</v>
       </c>
@@ -4726,7 +4709,7 @@
       <c r="E115" s="77"/>
       <c r="F115" s="57"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6">
       <c r="B116" s="74" t="s">
         <v>340</v>
       </c>
@@ -4737,7 +4720,7 @@
       <c r="E116" s="77"/>
       <c r="F116" s="57"/>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6">
       <c r="B117" s="74" t="s">
         <v>341</v>
       </c>
@@ -4748,7 +4731,7 @@
       <c r="E117" s="77"/>
       <c r="F117" s="57"/>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6">
       <c r="B118" s="74" t="s">
         <v>342</v>
       </c>
@@ -4759,7 +4742,7 @@
       <c r="E118" s="77"/>
       <c r="F118" s="57"/>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6">
       <c r="B119" s="74" t="s">
         <v>343</v>
       </c>
@@ -4770,14 +4753,14 @@
       <c r="E119" s="77"/>
       <c r="F119" s="57"/>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6">
       <c r="B120" s="74"/>
       <c r="C120" s="75"/>
       <c r="D120" s="76"/>
       <c r="E120" s="77"/>
       <c r="F120" s="57"/>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6">
       <c r="A121" s="53" t="s">
         <v>272</v>
       </c>
@@ -4787,7 +4770,7 @@
       <c r="E121" s="77"/>
       <c r="F121" s="57"/>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6">
       <c r="B122" s="74" t="s">
         <v>10</v>
       </c>
@@ -4798,7 +4781,7 @@
       <c r="E122" s="77"/>
       <c r="F122" s="57"/>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6">
       <c r="B123" s="74" t="s">
         <v>6</v>
       </c>
@@ -4809,7 +4792,7 @@
       <c r="E123" s="77"/>
       <c r="F123" s="57"/>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6">
       <c r="B124" s="74" t="s">
         <v>5</v>
       </c>
@@ -4820,7 +4803,7 @@
       <c r="E124" s="77"/>
       <c r="F124" s="57"/>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6">
       <c r="B125" s="74" t="s">
         <v>7</v>
       </c>
@@ -4831,7 +4814,7 @@
       <c r="E125" s="77"/>
       <c r="F125" s="57"/>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6">
       <c r="B126" s="74" t="s">
         <v>344</v>
       </c>
@@ -4842,7 +4825,7 @@
       <c r="E126" s="77"/>
       <c r="F126" s="57"/>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6">
       <c r="B127" s="74" t="s">
         <v>270</v>
       </c>
@@ -4853,7 +4836,7 @@
       <c r="E127" s="77"/>
       <c r="F127" s="57"/>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6">
       <c r="B128" s="74" t="s">
         <v>11</v>
       </c>
@@ -4864,7 +4847,7 @@
       <c r="E128" s="77"/>
       <c r="F128" s="57"/>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6">
       <c r="B129" s="74" t="s">
         <v>12</v>
       </c>
@@ -4875,7 +4858,7 @@
       <c r="E129" s="77"/>
       <c r="F129" s="57"/>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6">
       <c r="B130" s="74" t="s">
         <v>345</v>
       </c>
@@ -4886,7 +4869,7 @@
       <c r="E130" s="77"/>
       <c r="F130" s="57"/>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6">
       <c r="B131" s="74" t="s">
         <v>346</v>
       </c>
@@ -4897,21 +4880,21 @@
       <c r="E131" s="77"/>
       <c r="F131" s="57"/>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6">
       <c r="B132" s="74"/>
       <c r="C132" s="75"/>
       <c r="D132" s="76"/>
       <c r="E132" s="77"/>
       <c r="F132" s="57"/>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6">
       <c r="B133" s="74"/>
       <c r="C133" s="75"/>
       <c r="D133" s="76"/>
       <c r="E133" s="77"/>
       <c r="F133" s="57"/>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6">
       <c r="A134" s="53" t="s">
         <v>274</v>
       </c>
@@ -4921,7 +4904,7 @@
       <c r="E134" s="77"/>
       <c r="F134" s="57"/>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6">
       <c r="B135" s="74" t="s">
         <v>1</v>
       </c>
@@ -4932,7 +4915,7 @@
       <c r="E135" s="77"/>
       <c r="F135" s="57"/>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6">
       <c r="B136" s="74" t="s">
         <v>347</v>
       </c>
@@ -4943,7 +4926,7 @@
       <c r="E136" s="77"/>
       <c r="F136" s="57"/>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6">
       <c r="B137" s="74" t="s">
         <v>0</v>
       </c>
@@ -4954,7 +4937,7 @@
       <c r="E137" s="77"/>
       <c r="F137" s="57"/>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6">
       <c r="B138" s="74" t="s">
         <v>348</v>
       </c>
@@ -4965,7 +4948,7 @@
       <c r="E138" s="77"/>
       <c r="F138" s="57"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6">
       <c r="B139" s="74" t="s">
         <v>349</v>
       </c>
@@ -4976,7 +4959,7 @@
       <c r="E139" s="77"/>
       <c r="F139" s="57"/>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6">
       <c r="B140" s="74" t="s">
         <v>350</v>
       </c>
@@ -4987,14 +4970,14 @@
       <c r="E140" s="77"/>
       <c r="F140" s="57"/>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6">
       <c r="B141" s="74"/>
       <c r="C141" s="75"/>
       <c r="D141" s="76"/>
       <c r="E141" s="77"/>
       <c r="F141" s="57"/>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6">
       <c r="A142" s="53" t="s">
         <v>276</v>
       </c>
@@ -5004,7 +4987,7 @@
       <c r="E142" s="77"/>
       <c r="F142" s="57"/>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6">
       <c r="B143" s="74" t="s">
         <v>351</v>
       </c>
@@ -5015,7 +4998,7 @@
       <c r="E143" s="77"/>
       <c r="F143" s="57"/>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6">
       <c r="B144" s="74" t="s">
         <v>352</v>
       </c>
@@ -5026,7 +5009,7 @@
       <c r="E144" s="77"/>
       <c r="F144" s="57"/>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6">
       <c r="B145" s="74" t="s">
         <v>303</v>
       </c>
@@ -5037,7 +5020,7 @@
       <c r="E145" s="77"/>
       <c r="F145" s="57"/>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6">
       <c r="B146" s="74" t="s">
         <v>353</v>
       </c>
@@ -5048,7 +5031,7 @@
       <c r="E146" s="77"/>
       <c r="F146" s="57"/>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6">
       <c r="B147" s="74" t="s">
         <v>354</v>
       </c>
@@ -5059,7 +5042,7 @@
       <c r="E147" s="77"/>
       <c r="F147" s="57"/>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6">
       <c r="B148" s="74" t="s">
         <v>355</v>
       </c>
@@ -5070,7 +5053,7 @@
       <c r="E148" s="77"/>
       <c r="F148" s="57"/>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6">
       <c r="A149" s="53" t="s">
         <v>239</v>
       </c>
@@ -5080,7 +5063,7 @@
       <c r="E149" s="77"/>
       <c r="F149" s="57"/>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6">
       <c r="B150" s="74" t="s">
         <v>356</v>
       </c>
@@ -5091,7 +5074,7 @@
       <c r="E150" s="77"/>
       <c r="F150" s="57"/>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6">
       <c r="B151" s="74" t="s">
         <v>241</v>
       </c>
@@ -5102,7 +5085,7 @@
       <c r="E151" s="77"/>
       <c r="F151" s="57"/>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6">
       <c r="B152" s="74" t="s">
         <v>243</v>
       </c>
@@ -5113,7 +5096,7 @@
       <c r="E152" s="77"/>
       <c r="F152" s="57"/>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6">
       <c r="B153" s="74" t="s">
         <v>245</v>
       </c>
@@ -5124,7 +5107,7 @@
       <c r="E153" s="77"/>
       <c r="F153" s="57"/>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6">
       <c r="B154" s="74" t="s">
         <v>247</v>
       </c>
@@ -5135,7 +5118,7 @@
       <c r="E154" s="77"/>
       <c r="F154" s="57"/>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6">
       <c r="B155" s="74" t="s">
         <v>249</v>
       </c>
@@ -5146,42 +5129,42 @@
       <c r="E155" s="77"/>
       <c r="F155" s="57"/>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6">
       <c r="B156" s="74"/>
       <c r="C156" s="75"/>
       <c r="D156" s="76"/>
       <c r="E156" s="77"/>
       <c r="F156" s="57"/>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6">
       <c r="B157" s="74"/>
       <c r="C157" s="75"/>
       <c r="D157" s="76"/>
       <c r="E157" s="77"/>
       <c r="F157" s="57"/>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6">
       <c r="B158" s="74"/>
       <c r="C158" s="75"/>
       <c r="D158" s="76"/>
       <c r="E158" s="77"/>
       <c r="F158" s="57"/>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6">
       <c r="B159" s="74"/>
       <c r="C159" s="75"/>
       <c r="D159" s="76"/>
       <c r="E159" s="77"/>
       <c r="F159" s="57"/>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6">
       <c r="B160" s="74"/>
       <c r="C160" s="75"/>
       <c r="D160" s="76"/>
       <c r="E160" s="77"/>
       <c r="F160" s="57"/>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6">
       <c r="A162" s="110" t="s">
         <v>9</v>
       </c>
@@ -5201,7 +5184,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6">
       <c r="A163" s="111"/>
       <c r="B163" s="45" t="s">
         <v>251</v>
@@ -5215,7 +5198,7 @@
       </c>
       <c r="F163" s="57"/>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6">
       <c r="A164" s="111"/>
       <c r="B164" s="54" t="s">
         <v>254</v>
@@ -5229,7 +5212,7 @@
       </c>
       <c r="F164" s="57"/>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6">
       <c r="A165" s="111"/>
       <c r="B165" s="45" t="s">
         <v>256</v>
@@ -5243,7 +5226,7 @@
       </c>
       <c r="F165" s="57"/>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6">
       <c r="A166" s="111"/>
       <c r="B166" s="45" t="s">
         <v>258</v>
@@ -5257,58 +5240,58 @@
       </c>
       <c r="F166" s="57"/>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6">
       <c r="A168" s="84"/>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6">
       <c r="A169" s="84"/>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6">
       <c r="A170" s="84"/>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6">
       <c r="C171" s="85" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6">
       <c r="D172" s="86" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6">
       <c r="D173" s="86" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6">
       <c r="D174" s="86" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6">
       <c r="D175" s="87" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6">
       <c r="D176" s="47" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="177" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="4:5">
       <c r="D177" s="88"/>
       <c r="E177" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="178" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="4:5">
       <c r="D178" s="89"/>
       <c r="E178" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="179" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="4:5">
       <c r="D179" s="95"/>
       <c r="E179" t="s">
         <v>268</v>

</xml_diff>

<commit_message>
adding changes in examples
</commit_message>
<xml_diff>
--- a/my1stProject/apb_subsystem/apb_subsustem_design_arch.xlsx
+++ b/my1stProject/apb_subsystem/apb_subsustem_design_arch.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anupam\git\hello-world\my1stProject\apb_subsystem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anupam\Documents\SoCgit\hello-world\my1stProject\apb_subsystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="3" r:id="rId1"/>
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="443">
   <si>
     <t>Target</t>
   </si>
@@ -1606,12 +1606,15 @@
   <si>
     <t>find</t>
   </si>
+  <si>
+    <t>..\apbbus\apbbus.xlsx</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1751,6 +1754,14 @@
       <color theme="4" tint="-0.249977111117893"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -2184,10 +2195,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2473,18 +2485,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -2878,8 +2887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2966,7 +2975,9 @@
       <c r="G5" s="85"/>
       <c r="H5" s="85"/>
       <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
+      <c r="J5" s="119" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="85"/>
@@ -3751,8 +3762,11 @@
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:F1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="J5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3760,8 +3774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3798,8 +3812,8 @@
       <c r="D3" t="s">
         <v>441</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>371</v>
+      <c r="E3" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4079,12 +4093,12 @@
     <mergeCell ref="C1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="A6:XFD22">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
       <formula>$E$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>$E$3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4098,7 +4112,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>